<commit_message>
Send mission (waypoint) count as parameter id = 6 in 0x5007 Parameter frame
v0.16 2018-09-28  Send mission (waypoint) count as parameter id = 6 in 0x5007 Parameter frame
</commit_message>
<xml_diff>
--- a/Mavlink_Frsky_Passthru_Telemetry_Extended.xlsx
+++ b/Mavlink_Frsky_Passthru_Telemetry_Extended.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="177">
   <si>
     <t xml:space="preserve">Source</t>
   </si>
@@ -397,6 +397,15 @@
     <t xml:space="preserve">centi Volts (Vx100)</t>
   </si>
   <si>
+    <t xml:space="preserve">5.battery pack 2 capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.number of waypoints in mission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number</t>
+  </si>
+  <si>
     <t xml:space="preserve">ParamId   1,2,3,4....</t>
   </si>
   <si>
@@ -466,7 +475,7 @@
     <t xml:space="preserve">Fragment 4 sign bit</t>
   </si>
   <si>
-    <t xml:space="preserve">0x5010</t>
+    <t xml:space="preserve">0x500A</t>
   </si>
   <si>
     <t xml:space="preserve">HUD</t>
@@ -493,10 +502,10 @@
     <t xml:space="preserve">18-27</t>
   </si>
   <si>
-    <t xml:space="preserve">0x5011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mission</t>
+    <t xml:space="preserve">0x500B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Missions</t>
   </si>
   <si>
     <t xml:space="preserve">WP Number</t>
@@ -520,7 +529,7 @@
     <t xml:space="preserve">24-29</t>
   </si>
   <si>
-    <t xml:space="preserve">WP bearing offset from yaw</t>
+    <t xml:space="preserve">Next WP bearing offset from “nav_bearing” in AP</t>
   </si>
   <si>
     <t xml:space="preserve">45 degrees</t>
@@ -529,7 +538,7 @@
     <t xml:space="preserve">30-32</t>
   </si>
   <si>
-    <t xml:space="preserve">0x5012</t>
+    <t xml:space="preserve">0x500C</t>
   </si>
   <si>
     <t xml:space="preserve">Wind Estimate</t>
@@ -1165,10 +1174,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H103"/>
+  <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F76" activeCellId="0" sqref="F:F"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M47" activeCellId="0" sqref="M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1177,7 +1186,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.18"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.26"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
@@ -2348,211 +2357,213 @@
       <c r="G64" s="60"/>
       <c r="H64" s="57"/>
     </row>
-    <row r="65" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="29"/>
       <c r="B65" s="30"/>
-      <c r="C65" s="32"/>
-      <c r="D65" s="32"/>
-      <c r="E65" s="32"/>
+      <c r="C65" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="D65" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E65" s="17" t="n">
+        <v>24</v>
+      </c>
       <c r="F65" s="32"/>
       <c r="G65" s="23"/>
       <c r="H65" s="33"/>
     </row>
-    <row r="66" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="29"/>
       <c r="B66" s="30"/>
-      <c r="C66" s="32" t="s">
-        <v>125</v>
-      </c>
-      <c r="D66" s="32"/>
-      <c r="E66" s="32" t="n">
-        <v>4</v>
+      <c r="C66" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="D66" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="E66" s="17" t="n">
+        <v>24</v>
       </c>
       <c r="F66" s="32"/>
-      <c r="G66" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="H66" s="33" t="n">
-        <v>24</v>
-      </c>
+      <c r="G66" s="23"/>
+      <c r="H66" s="33"/>
     </row>
     <row r="67" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="29"/>
       <c r="B67" s="30"/>
-      <c r="C67" s="32"/>
+      <c r="C67" s="32" t="s">
+        <v>128</v>
+      </c>
       <c r="D67" s="32"/>
-      <c r="E67" s="32"/>
+      <c r="E67" s="32" t="n">
+        <v>4</v>
+      </c>
       <c r="F67" s="32"/>
       <c r="G67" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="H67" s="33" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="29"/>
+      <c r="B68" s="30"/>
+      <c r="C68" s="32"/>
+      <c r="D68" s="32"/>
+      <c r="E68" s="32"/>
+      <c r="F68" s="32"/>
+      <c r="G68" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H67" s="33"/>
-    </row>
-    <row r="68" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="24"/>
-      <c r="B68" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="C68" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="D68" s="26"/>
-      <c r="E68" s="26"/>
-      <c r="F68" s="26"/>
-      <c r="G68" s="27"/>
-      <c r="H68" s="37" t="s">
+      <c r="H68" s="33"/>
+    </row>
+    <row r="69" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="24"/>
+      <c r="B69" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="C69" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="D69" s="26"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="26"/>
+      <c r="G69" s="27"/>
+      <c r="H69" s="37" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="29"/>
-      <c r="B69" s="30"/>
-      <c r="C69" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D69" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="E69" s="32" t="n">
-        <v>9</v>
-      </c>
-      <c r="F69" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="G69" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="H69" s="33" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="29"/>
       <c r="B70" s="30"/>
-      <c r="C70" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="D70" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E70" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="F70" s="32"/>
-      <c r="G70" s="23" t="n">
-        <v>10</v>
+      <c r="C70" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D70" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E70" s="32" t="n">
+        <v>9</v>
+      </c>
+      <c r="F70" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G70" s="23" t="s">
+        <v>74</v>
       </c>
       <c r="H70" s="33" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="29"/>
       <c r="B71" s="30"/>
-      <c r="C71" s="45"/>
-      <c r="D71" s="32" t="s">
+      <c r="C71" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="D71" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E71" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F71" s="32"/>
+      <c r="G71" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="H71" s="33" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="29"/>
+      <c r="B72" s="30"/>
+      <c r="C72" s="45"/>
+      <c r="D72" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="E71" s="17" t="n">
+      <c r="E72" s="17" t="n">
         <v>7</v>
       </c>
-      <c r="F71" s="32"/>
-      <c r="G71" s="23" t="s">
+      <c r="F72" s="32"/>
+      <c r="G72" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="H71" s="33" t="n">
+      <c r="H72" s="33" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="46"/>
-      <c r="B72" s="47"/>
-      <c r="C72" s="17" t="s">
+    <row r="73" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="46"/>
+      <c r="B73" s="47"/>
+      <c r="C73" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D72" s="17" t="s">
+      <c r="D73" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E72" s="17" t="n">
+      <c r="E73" s="17" t="n">
         <v>15</v>
       </c>
-      <c r="F72" s="17" t="s">
+      <c r="F73" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="G72" s="23" t="s">
+      <c r="G73" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="H72" s="33" t="n">
+      <c r="H73" s="33" t="n">
         <v>17</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="29"/>
-      <c r="B73" s="30"/>
-      <c r="C73" s="32"/>
-      <c r="D73" s="32"/>
-      <c r="E73" s="32"/>
-      <c r="G73" s="23" t="s">
+    <row r="74" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="29"/>
+      <c r="B74" s="30"/>
+      <c r="C74" s="32"/>
+      <c r="D74" s="32"/>
+      <c r="E74" s="32"/>
+      <c r="G74" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H73" s="33"/>
-    </row>
-    <row r="74" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="B74" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="C74" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="D74" s="26"/>
-      <c r="E74" s="26"/>
-      <c r="F74" s="26"/>
-      <c r="G74" s="27"/>
-      <c r="H74" s="37" t="s">
+      <c r="H74" s="33"/>
+    </row>
+    <row r="75" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B75" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="C75" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="D75" s="26"/>
+      <c r="E75" s="26"/>
+      <c r="F75" s="26"/>
+      <c r="G75" s="27"/>
+      <c r="H75" s="37" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="29"/>
-      <c r="B75" s="30"/>
-      <c r="C75" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="D75" s="32"/>
-      <c r="E75" s="32" t="n">
-        <v>4</v>
-      </c>
-      <c r="F75" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="G75" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="H75" s="33" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="29"/>
       <c r="B76" s="30"/>
-      <c r="C76" s="32" t="s">
-        <v>134</v>
+      <c r="C76" s="0" t="s">
+        <v>135</v>
       </c>
       <c r="D76" s="32"/>
       <c r="E76" s="32" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F76" s="32" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G76" s="23" t="s">
-        <v>136</v>
+        <v>52</v>
       </c>
       <c r="H76" s="33" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2563,252 +2574,254 @@
       </c>
       <c r="D77" s="32"/>
       <c r="E77" s="32" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F77" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="G77" s="23" t="n">
-        <v>11</v>
+      <c r="G77" s="23" t="s">
+        <v>139</v>
       </c>
       <c r="H77" s="33" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="29"/>
       <c r="B78" s="30"/>
       <c r="C78" s="32" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D78" s="32"/>
       <c r="E78" s="32" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F78" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="G78" s="23" t="s">
-        <v>140</v>
+        <v>141</v>
+      </c>
+      <c r="G78" s="23" t="n">
+        <v>11</v>
       </c>
       <c r="H78" s="33" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="29"/>
       <c r="B79" s="30"/>
       <c r="C79" s="32" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D79" s="32"/>
       <c r="E79" s="32" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F79" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="G79" s="23" t="n">
-        <v>18</v>
+      <c r="G79" s="23" t="s">
+        <v>143</v>
       </c>
       <c r="H79" s="33" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="29"/>
       <c r="B80" s="30"/>
       <c r="C80" s="32" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D80" s="32"/>
       <c r="E80" s="32" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F80" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="G80" s="23" t="s">
-        <v>143</v>
+        <v>141</v>
+      </c>
+      <c r="G80" s="23" t="n">
+        <v>18</v>
       </c>
       <c r="H80" s="33" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="29"/>
       <c r="B81" s="30"/>
       <c r="C81" s="32" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D81" s="32"/>
       <c r="E81" s="32" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F81" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="G81" s="23" t="n">
-        <v>25</v>
+      <c r="G81" s="23" t="s">
+        <v>146</v>
       </c>
       <c r="H81" s="33" t="n">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="29"/>
       <c r="B82" s="30"/>
       <c r="C82" s="32" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D82" s="32"/>
       <c r="E82" s="32" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F82" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="G82" s="23" t="s">
-        <v>146</v>
+        <v>141</v>
+      </c>
+      <c r="G82" s="23" t="n">
+        <v>25</v>
       </c>
       <c r="H82" s="33" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="29"/>
       <c r="B83" s="30"/>
       <c r="C83" s="32" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D83" s="32"/>
       <c r="E83" s="32" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F83" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="G83" s="23" t="n">
+      <c r="G83" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="H83" s="33" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="29"/>
+      <c r="B84" s="30"/>
+      <c r="C84" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="D84" s="32"/>
+      <c r="E84" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="F84" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="G84" s="23" t="n">
         <v>32</v>
       </c>
-      <c r="H83" s="33" t="n">
+      <c r="H84" s="33" t="n">
         <v>31</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="24" t="s">
+    <row r="85" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="B84" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="C84" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="D84" s="26"/>
-      <c r="E84" s="26"/>
-      <c r="F84" s="26"/>
-      <c r="G84" s="27" t="s">
+      <c r="B85" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="C85" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="D85" s="26"/>
+      <c r="E85" s="26"/>
+      <c r="F85" s="26"/>
+      <c r="G85" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="H84" s="37" t="s">
+      <c r="H85" s="37" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="29"/>
-      <c r="B85" s="30"/>
-      <c r="C85" s="45" t="s">
-        <v>150</v>
-      </c>
-      <c r="D85" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E85" s="32" t="n">
-        <v>1</v>
-      </c>
-      <c r="F85" s="32"/>
-      <c r="G85" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="H85" s="33" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="29"/>
       <c r="B86" s="30"/>
-      <c r="C86" s="45"/>
-      <c r="D86" s="32" t="s">
-        <v>99</v>
+      <c r="C86" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="D86" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="E86" s="32" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F86" s="32"/>
-      <c r="G86" s="23" t="s">
-        <v>100</v>
+      <c r="G86" s="23" t="n">
+        <v>1</v>
       </c>
       <c r="H86" s="33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="29"/>
       <c r="B87" s="30"/>
-      <c r="C87" s="32" t="s">
-        <v>151</v>
-      </c>
-      <c r="D87" s="32"/>
+      <c r="C87" s="45"/>
+      <c r="D87" s="32" t="s">
+        <v>99</v>
+      </c>
       <c r="E87" s="32" t="n">
         <v>7</v>
       </c>
-      <c r="F87" s="32" t="s">
-        <v>152</v>
-      </c>
+      <c r="F87" s="32"/>
       <c r="G87" s="23" t="s">
-        <v>153</v>
+        <v>100</v>
       </c>
       <c r="H87" s="33" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="29"/>
       <c r="B88" s="30"/>
-      <c r="C88" s="45" t="s">
+      <c r="C88" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="D88" s="17" t="s">
-        <v>57</v>
-      </c>
+      <c r="D88" s="32"/>
       <c r="E88" s="32" t="n">
-        <v>2</v>
-      </c>
-      <c r="F88" s="32"/>
+        <v>7</v>
+      </c>
+      <c r="F88" s="32" t="s">
+        <v>155</v>
+      </c>
       <c r="G88" s="23" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H88" s="33" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="29"/>
       <c r="B89" s="30"/>
-      <c r="C89" s="45"/>
-      <c r="D89" s="32" t="s">
-        <v>58</v>
+      <c r="C89" s="45" t="s">
+        <v>157</v>
+      </c>
+      <c r="D89" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="E89" s="32" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F89" s="32"/>
       <c r="G89" s="23" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H89" s="33" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2816,220 +2829,238 @@
       <c r="B90" s="30"/>
       <c r="C90" s="45"/>
       <c r="D90" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E90" s="32" t="n">
+        <v>10</v>
+      </c>
+      <c r="F90" s="32"/>
+      <c r="G90" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="H90" s="33" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="29"/>
+      <c r="B91" s="30"/>
+      <c r="C91" s="45"/>
+      <c r="D91" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="E90" s="32" t="n">
+      <c r="E91" s="32" t="n">
         <v>1</v>
       </c>
-      <c r="F90" s="52"/>
-      <c r="G90" s="23" t="n">
+      <c r="F91" s="52"/>
+      <c r="G91" s="23" t="n">
         <v>28</v>
       </c>
-      <c r="H90" s="33" t="n">
+      <c r="H91" s="33" t="n">
         <v>27</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="61"/>
-      <c r="B91" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="C91" s="26" t="s">
-        <v>158</v>
-      </c>
-      <c r="D91" s="26"/>
-      <c r="E91" s="26"/>
-      <c r="F91" s="26"/>
-      <c r="G91" s="27"/>
-      <c r="H91" s="37" t="s">
+    <row r="92" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="61"/>
+      <c r="B92" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="C92" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="D92" s="26"/>
+      <c r="E92" s="26"/>
+      <c r="F92" s="26"/>
+      <c r="G92" s="27"/>
+      <c r="H92" s="37" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="62"/>
-      <c r="C92" s="63" t="s">
-        <v>159</v>
-      </c>
-      <c r="D92" s="63"/>
-      <c r="E92" s="63" t="n">
+    <row r="93" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="62"/>
+      <c r="C93" s="63" t="s">
+        <v>162</v>
+      </c>
+      <c r="D93" s="63"/>
+      <c r="E93" s="63" t="n">
         <v>10</v>
       </c>
-      <c r="F92" s="63"/>
-      <c r="G92" s="64" t="s">
-        <v>160</v>
-      </c>
-      <c r="H92" s="65" t="n">
+      <c r="F93" s="63"/>
+      <c r="G93" s="64" t="s">
+        <v>163</v>
+      </c>
+      <c r="H93" s="65" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="66"/>
-      <c r="C93" s="67" t="s">
-        <v>161</v>
-      </c>
-      <c r="D93" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E93" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G93" s="68" t="s">
-        <v>39</v>
-      </c>
-      <c r="H93" s="8" t="n">
-        <v>10</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="66"/>
-      <c r="C94" s="67"/>
+      <c r="C94" s="67" t="s">
+        <v>164</v>
+      </c>
       <c r="D94" s="0" t="s">
-        <v>162</v>
+        <v>57</v>
       </c>
       <c r="E94" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G94" s="68" t="s">
+        <v>39</v>
+      </c>
+      <c r="H94" s="8" t="n">
         <v>10</v>
-      </c>
-      <c r="G94" s="68" t="s">
-        <v>163</v>
-      </c>
-      <c r="H94" s="8" t="n">
-        <v>12</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="66"/>
-      <c r="C95" s="67" t="s">
-        <v>164</v>
-      </c>
+      <c r="C95" s="67"/>
       <c r="D95" s="0" t="s">
-        <v>57</v>
+        <v>165</v>
       </c>
       <c r="E95" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G95" s="68" t="n">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="G95" s="68" t="s">
+        <v>166</v>
       </c>
       <c r="H95" s="8" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="66"/>
-      <c r="C96" s="67"/>
+      <c r="C96" s="67" t="s">
+        <v>167</v>
+      </c>
       <c r="D96" s="0" t="s">
-        <v>162</v>
+        <v>57</v>
       </c>
       <c r="E96" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G96" s="68" t="s">
-        <v>165</v>
+        <v>1</v>
+      </c>
+      <c r="G96" s="68" t="n">
+        <v>23</v>
       </c>
       <c r="H96" s="8" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="66"/>
-      <c r="C97" s="69" t="s">
-        <v>166</v>
-      </c>
+      <c r="C97" s="67"/>
       <c r="D97" s="0" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E97" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G97" s="68" t="s">
         <v>168</v>
       </c>
       <c r="H97" s="8" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="66"/>
-      <c r="G98" s="68"/>
-      <c r="H98" s="8"/>
+      <c r="C98" s="69" t="s">
+        <v>169</v>
+      </c>
+      <c r="D98" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="E98" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G98" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="H98" s="8" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="70"/>
-      <c r="B99" s="71" t="s">
-        <v>169</v>
-      </c>
-      <c r="C99" s="71" t="s">
-        <v>170</v>
-      </c>
-      <c r="D99" s="71"/>
-      <c r="E99" s="71"/>
-      <c r="F99" s="71"/>
-      <c r="G99" s="72"/>
-      <c r="H99" s="73"/>
+      <c r="A99" s="66"/>
+      <c r="G99" s="68"/>
+      <c r="H99" s="8"/>
     </row>
     <row r="100" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="62"/>
-      <c r="B100" s="63"/>
-      <c r="C100" s="74" t="s">
-        <v>171</v>
-      </c>
-      <c r="D100" s="0" t="s">
+      <c r="A100" s="70"/>
+      <c r="B100" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="C100" s="71" t="s">
+        <v>173</v>
+      </c>
+      <c r="D100" s="71"/>
+      <c r="E100" s="71"/>
+      <c r="F100" s="71"/>
+      <c r="G100" s="72"/>
+      <c r="H100" s="73"/>
+    </row>
+    <row r="101" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="62"/>
+      <c r="B101" s="63"/>
+      <c r="C101" s="74" t="s">
+        <v>174</v>
+      </c>
+      <c r="D101" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="E100" s="63" t="n">
+      <c r="E101" s="63" t="n">
         <v>1</v>
       </c>
-      <c r="F100" s="63"/>
-      <c r="G100" s="64" t="n">
+      <c r="F101" s="63"/>
+      <c r="G101" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="H100" s="65" t="n">
+      <c r="H101" s="65" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="66"/>
-      <c r="C101" s="74"/>
-      <c r="D101" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="E101" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="G101" s="68" t="s">
-        <v>100</v>
-      </c>
-      <c r="H101" s="8" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="66"/>
-      <c r="C102" s="0" t="s">
-        <v>173</v>
-      </c>
+      <c r="C102" s="74"/>
       <c r="D102" s="0" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="E102" s="0" t="n">
         <v>7</v>
       </c>
       <c r="G102" s="68" t="s">
-        <v>153</v>
+        <v>100</v>
       </c>
       <c r="H102" s="8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="66"/>
+      <c r="C103" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="D103" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E103" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G103" s="68" t="s">
+        <v>156</v>
+      </c>
+      <c r="H103" s="8" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="75"/>
-      <c r="B103" s="76"/>
-      <c r="C103" s="76"/>
-      <c r="D103" s="76"/>
-      <c r="E103" s="76"/>
-      <c r="F103" s="76"/>
-      <c r="G103" s="77"/>
-      <c r="H103" s="78"/>
+    <row r="104" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="75"/>
+      <c r="B104" s="76"/>
+      <c r="C104" s="76"/>
+      <c r="D104" s="76"/>
+      <c r="E104" s="76"/>
+      <c r="F104" s="76"/>
+      <c r="G104" s="77"/>
+      <c r="H104" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -3043,12 +3074,12 @@
     <mergeCell ref="C47:C49"/>
     <mergeCell ref="C50:C51"/>
     <mergeCell ref="C57:C58"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="C88:C90"/>
-    <mergeCell ref="C93:C94"/>
-    <mergeCell ref="C95:C96"/>
-    <mergeCell ref="C100:C101"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="C89:C91"/>
+    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="C101:C102"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Re-arrange our custom message IDs as per Alex's request
</commit_message>
<xml_diff>
--- a/Mavlink_Frsky_Passthru_Telemetry_Extended.xlsx
+++ b/Mavlink_Frsky_Passthru_Telemetry_Extended.xlsx
@@ -418,10 +418,46 @@
     <t xml:space="preserve">Battery 2</t>
   </si>
   <si>
+    <t xml:space="preserve">0x5009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Missions/Waypoints</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WP Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distance to next waypoint (0-102km)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xtrack error (0m – 31m, 10m – 310m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24-29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Next WP bearing offset from “nav_bearing” in AP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45 degrees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30-32</t>
+  </si>
+  <si>
     <t xml:space="preserve">#65</t>
   </si>
   <si>
-    <t xml:space="preserve">0x5009</t>
+    <t xml:space="preserve">0x50F1</t>
   </si>
   <si>
     <t xml:space="preserve">Servo Channels</t>
@@ -475,10 +511,10 @@
     <t xml:space="preserve">Fragment 4 sign bit</t>
   </si>
   <si>
-    <t xml:space="preserve">0x500A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HUD</t>
+    <t xml:space="preserve">0x50F2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VFR HUD</t>
   </si>
   <si>
     <t xml:space="preserve">Airspeed</t>
@@ -502,43 +538,7 @@
     <t xml:space="preserve">18-27</t>
   </si>
   <si>
-    <t xml:space="preserve">0x500B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Missions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WP Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distance to next waypoint (0-102km)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">metres</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13-22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xtrack error (0m – 31m, 10m – 310m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24-29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Next WP bearing offset from “nav_bearing” in AP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45 degrees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30-32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x500C</t>
+    <t xml:space="preserve">0x50F3</t>
   </si>
   <si>
     <t xml:space="preserve">Wind Estimate</t>
@@ -1099,12 +1099,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1174,10 +1174,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H104"/>
+  <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M47" activeCellId="0" sqref="M47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A63" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B104" activeCellId="0" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2529,14 +2529,12 @@
       <c r="H74" s="33"/>
     </row>
     <row r="75" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="24" t="s">
+      <c r="A75" s="61"/>
+      <c r="B75" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="B75" s="25" t="s">
+      <c r="C75" s="26" t="s">
         <v>133</v>
-      </c>
-      <c r="C75" s="26" t="s">
-        <v>134</v>
       </c>
       <c r="D75" s="26"/>
       <c r="E75" s="26"/>
@@ -2546,521 +2544,539 @@
         <v>48</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="29"/>
-      <c r="B76" s="30"/>
-      <c r="C76" s="0" t="s">
+    <row r="76" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="62"/>
+      <c r="C76" s="63" t="s">
+        <v>134</v>
+      </c>
+      <c r="D76" s="63"/>
+      <c r="E76" s="63" t="n">
+        <v>10</v>
+      </c>
+      <c r="F76" s="63"/>
+      <c r="G76" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="D76" s="32"/>
-      <c r="E76" s="32" t="n">
-        <v>4</v>
-      </c>
-      <c r="F76" s="32" t="s">
+      <c r="H76" s="65" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="66"/>
+      <c r="C77" s="67" t="s">
         <v>136</v>
       </c>
-      <c r="G76" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="H76" s="33" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="29"/>
-      <c r="B77" s="30"/>
-      <c r="C77" s="32" t="s">
+      <c r="D77" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G77" s="68" t="s">
+        <v>39</v>
+      </c>
+      <c r="H77" s="8" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="66"/>
+      <c r="C78" s="67"/>
+      <c r="D78" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="D77" s="32"/>
-      <c r="E77" s="32" t="n">
-        <v>6</v>
-      </c>
-      <c r="F77" s="32" t="s">
+      <c r="E78" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G78" s="68" t="s">
         <v>138</v>
       </c>
-      <c r="G77" s="23" t="s">
+      <c r="H78" s="8" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="66"/>
+      <c r="C79" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="H77" s="33" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="29"/>
-      <c r="B78" s="30"/>
-      <c r="C78" s="32" t="s">
+      <c r="D79" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G79" s="68" t="n">
+        <v>23</v>
+      </c>
+      <c r="H79" s="8" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="66"/>
+      <c r="C80" s="67"/>
+      <c r="D80" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G80" s="68" t="s">
         <v>140</v>
       </c>
-      <c r="D78" s="32"/>
-      <c r="E78" s="32" t="n">
-        <v>1</v>
-      </c>
-      <c r="F78" s="32" t="s">
+      <c r="H80" s="8" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="66"/>
+      <c r="C81" s="69" t="s">
         <v>141</v>
       </c>
-      <c r="G78" s="23" t="n">
-        <v>11</v>
-      </c>
-      <c r="H78" s="33" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="29"/>
-      <c r="B79" s="30"/>
-      <c r="C79" s="32" t="s">
+      <c r="D81" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="D79" s="32"/>
-      <c r="E79" s="32" t="n">
-        <v>6</v>
-      </c>
-      <c r="F79" s="32" t="s">
-        <v>138</v>
-      </c>
-      <c r="G79" s="23" t="s">
+      <c r="E81" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G81" s="68" t="s">
         <v>143</v>
       </c>
-      <c r="H79" s="33" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="29"/>
-      <c r="B80" s="30"/>
-      <c r="C80" s="32" t="s">
+      <c r="H81" s="8" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="66"/>
+      <c r="C82" s="69"/>
+      <c r="G82" s="68"/>
+      <c r="H82" s="8"/>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="D80" s="32"/>
-      <c r="E80" s="32" t="n">
-        <v>1</v>
-      </c>
-      <c r="F80" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="G80" s="23" t="n">
-        <v>18</v>
-      </c>
-      <c r="H80" s="33" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="29"/>
-      <c r="B81" s="30"/>
-      <c r="C81" s="32" t="s">
+      <c r="B83" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="D81" s="32"/>
-      <c r="E81" s="32" t="n">
-        <v>6</v>
-      </c>
-      <c r="F81" s="32" t="s">
-        <v>138</v>
-      </c>
-      <c r="G81" s="23" t="s">
+      <c r="C83" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="H81" s="33" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="29"/>
-      <c r="B82" s="30"/>
-      <c r="C82" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="D82" s="32"/>
-      <c r="E82" s="32" t="n">
-        <v>1</v>
-      </c>
-      <c r="F82" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="G82" s="23" t="n">
-        <v>25</v>
-      </c>
-      <c r="H82" s="33" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="29"/>
-      <c r="B83" s="30"/>
-      <c r="C83" s="32" t="s">
-        <v>148</v>
-      </c>
-      <c r="D83" s="32"/>
-      <c r="E83" s="32" t="n">
-        <v>6</v>
-      </c>
-      <c r="F83" s="32" t="s">
-        <v>138</v>
-      </c>
-      <c r="G83" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="H83" s="33" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D83" s="26"/>
+      <c r="E83" s="26"/>
+      <c r="F83" s="26"/>
+      <c r="G83" s="27"/>
+      <c r="H83" s="37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="29"/>
       <c r="B84" s="30"/>
-      <c r="C84" s="32" t="s">
-        <v>150</v>
+      <c r="C84" s="0" t="s">
+        <v>147</v>
       </c>
       <c r="D84" s="32"/>
       <c r="E84" s="32" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F84" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="G84" s="23" t="n">
-        <v>32</v>
+        <v>148</v>
+      </c>
+      <c r="G84" s="23" t="s">
+        <v>52</v>
       </c>
       <c r="H84" s="33" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="B85" s="25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="29"/>
+      <c r="B85" s="30"/>
+      <c r="C85" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="D85" s="32"/>
+      <c r="E85" s="32" t="n">
+        <v>6</v>
+      </c>
+      <c r="F85" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="G85" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="C85" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="D85" s="26"/>
-      <c r="E85" s="26"/>
-      <c r="F85" s="26"/>
-      <c r="G85" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="H85" s="37" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H85" s="33" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="29"/>
       <c r="B86" s="30"/>
-      <c r="C86" s="45" t="s">
-        <v>153</v>
-      </c>
-      <c r="D86" s="17" t="s">
-        <v>57</v>
-      </c>
+      <c r="C86" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="D86" s="32"/>
       <c r="E86" s="32" t="n">
         <v>1</v>
       </c>
-      <c r="F86" s="32"/>
+      <c r="F86" s="32" t="s">
+        <v>153</v>
+      </c>
       <c r="G86" s="23" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H86" s="33" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="29"/>
       <c r="B87" s="30"/>
-      <c r="C87" s="45"/>
-      <c r="D87" s="32" t="s">
-        <v>99</v>
-      </c>
+      <c r="C87" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="D87" s="32"/>
       <c r="E87" s="32" t="n">
-        <v>7</v>
-      </c>
-      <c r="F87" s="32"/>
+        <v>6</v>
+      </c>
+      <c r="F87" s="32" t="s">
+        <v>150</v>
+      </c>
       <c r="G87" s="23" t="s">
-        <v>100</v>
+        <v>155</v>
       </c>
       <c r="H87" s="33" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="29"/>
       <c r="B88" s="30"/>
       <c r="C88" s="32" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D88" s="32"/>
       <c r="E88" s="32" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F88" s="32" t="s">
-        <v>155</v>
-      </c>
-      <c r="G88" s="23" t="s">
-        <v>156</v>
+        <v>153</v>
+      </c>
+      <c r="G88" s="23" t="n">
+        <v>18</v>
       </c>
       <c r="H88" s="33" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="29"/>
       <c r="B89" s="30"/>
-      <c r="C89" s="45" t="s">
+      <c r="C89" s="32" t="s">
         <v>157</v>
       </c>
-      <c r="D89" s="17" t="s">
-        <v>57</v>
-      </c>
+      <c r="D89" s="32"/>
       <c r="E89" s="32" t="n">
-        <v>2</v>
-      </c>
-      <c r="F89" s="32"/>
+        <v>6</v>
+      </c>
+      <c r="F89" s="32" t="s">
+        <v>150</v>
+      </c>
       <c r="G89" s="23" t="s">
         <v>158</v>
       </c>
       <c r="H89" s="33" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="29"/>
       <c r="B90" s="30"/>
-      <c r="C90" s="45"/>
-      <c r="D90" s="32" t="s">
-        <v>58</v>
-      </c>
+      <c r="C90" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="D90" s="32"/>
       <c r="E90" s="32" t="n">
-        <v>10</v>
-      </c>
-      <c r="F90" s="32"/>
-      <c r="G90" s="23" t="s">
-        <v>159</v>
+        <v>1</v>
+      </c>
+      <c r="F90" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="G90" s="23" t="n">
+        <v>25</v>
       </c>
       <c r="H90" s="33" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="29"/>
       <c r="B91" s="30"/>
-      <c r="C91" s="45"/>
-      <c r="D91" s="32" t="s">
+      <c r="C91" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="D91" s="32"/>
+      <c r="E91" s="32" t="n">
+        <v>6</v>
+      </c>
+      <c r="F91" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="G91" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="H91" s="33" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="29"/>
+      <c r="B92" s="30"/>
+      <c r="C92" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="D92" s="32"/>
+      <c r="E92" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="F92" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="G92" s="23" t="n">
+        <v>32</v>
+      </c>
+      <c r="H92" s="33" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="29"/>
+      <c r="B93" s="30"/>
+      <c r="C93" s="32"/>
+      <c r="D93" s="32"/>
+      <c r="E93" s="32"/>
+      <c r="F93" s="32"/>
+      <c r="G93" s="23"/>
+      <c r="H93" s="33"/>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B94" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="C94" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="D94" s="26"/>
+      <c r="E94" s="26"/>
+      <c r="F94" s="26"/>
+      <c r="G94" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="H94" s="37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="29"/>
+      <c r="B95" s="30"/>
+      <c r="C95" s="45" t="s">
+        <v>165</v>
+      </c>
+      <c r="D95" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E95" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="F95" s="32"/>
+      <c r="G95" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="H95" s="33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="29"/>
+      <c r="B96" s="30"/>
+      <c r="C96" s="45"/>
+      <c r="D96" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="E96" s="32" t="n">
+        <v>7</v>
+      </c>
+      <c r="F96" s="32"/>
+      <c r="G96" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="H96" s="33" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="29"/>
+      <c r="B97" s="30"/>
+      <c r="C97" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="D97" s="32"/>
+      <c r="E97" s="32" t="n">
+        <v>7</v>
+      </c>
+      <c r="F97" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="G97" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="H97" s="33" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="29"/>
+      <c r="B98" s="30"/>
+      <c r="C98" s="45" t="s">
+        <v>169</v>
+      </c>
+      <c r="D98" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E98" s="32" t="n">
+        <v>2</v>
+      </c>
+      <c r="F98" s="32"/>
+      <c r="G98" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="H98" s="33" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="29"/>
+      <c r="B99" s="30"/>
+      <c r="C99" s="45"/>
+      <c r="D99" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E99" s="32" t="n">
+        <v>10</v>
+      </c>
+      <c r="F99" s="32"/>
+      <c r="G99" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="H99" s="33" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="29"/>
+      <c r="B100" s="30"/>
+      <c r="C100" s="45"/>
+      <c r="D100" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="E91" s="32" t="n">
+      <c r="E100" s="32" t="n">
         <v>1</v>
       </c>
-      <c r="F91" s="52"/>
-      <c r="G91" s="23" t="n">
+      <c r="F100" s="52"/>
+      <c r="G100" s="23" t="n">
         <v>28</v>
       </c>
-      <c r="H91" s="33" t="n">
+      <c r="H100" s="33" t="n">
         <v>27</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="61"/>
-      <c r="B92" s="26" t="s">
-        <v>160</v>
-      </c>
-      <c r="C92" s="26" t="s">
-        <v>161</v>
-      </c>
-      <c r="D92" s="26"/>
-      <c r="E92" s="26"/>
-      <c r="F92" s="26"/>
-      <c r="G92" s="27"/>
-      <c r="H92" s="37" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="62"/>
-      <c r="C93" s="63" t="s">
-        <v>162</v>
-      </c>
-      <c r="D93" s="63"/>
-      <c r="E93" s="63" t="n">
-        <v>10</v>
-      </c>
-      <c r="F93" s="63"/>
-      <c r="G93" s="64" t="s">
-        <v>163</v>
-      </c>
-      <c r="H93" s="65" t="n">
+    <row r="101" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="66"/>
+      <c r="G101" s="68"/>
+      <c r="H101" s="8"/>
+    </row>
+    <row r="102" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="70"/>
+      <c r="B102" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="C102" s="71" t="s">
+        <v>173</v>
+      </c>
+      <c r="D102" s="71"/>
+      <c r="E102" s="71"/>
+      <c r="F102" s="71"/>
+      <c r="G102" s="72"/>
+      <c r="H102" s="73"/>
+    </row>
+    <row r="103" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="62"/>
+      <c r="B103" s="63"/>
+      <c r="C103" s="74" t="s">
+        <v>174</v>
+      </c>
+      <c r="D103" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E103" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="F103" s="63"/>
+      <c r="G103" s="64" t="n">
+        <v>1</v>
+      </c>
+      <c r="H103" s="65" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="66"/>
-      <c r="C94" s="67" t="s">
-        <v>164</v>
-      </c>
-      <c r="D94" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E94" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G94" s="68" t="s">
-        <v>39</v>
-      </c>
-      <c r="H94" s="8" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="66"/>
-      <c r="C95" s="67"/>
-      <c r="D95" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="E95" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="G95" s="68" t="s">
-        <v>166</v>
-      </c>
-      <c r="H95" s="8" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="66"/>
-      <c r="C96" s="67" t="s">
-        <v>167</v>
-      </c>
-      <c r="D96" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E96" s="0" t="n">
+    <row r="104" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="66"/>
+      <c r="C104" s="74"/>
+      <c r="D104" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="E104" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G104" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="H104" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="G96" s="68" t="n">
-        <v>23</v>
-      </c>
-      <c r="H96" s="8" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="66"/>
-      <c r="C97" s="67"/>
-      <c r="D97" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="E97" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G97" s="68" t="s">
+    </row>
+    <row r="105" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="66"/>
+      <c r="C105" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="D105" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E105" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G105" s="68" t="s">
         <v>168</v>
       </c>
-      <c r="H97" s="8" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="66"/>
-      <c r="C98" s="69" t="s">
-        <v>169</v>
-      </c>
-      <c r="D98" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="E98" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="G98" s="68" t="s">
-        <v>171</v>
-      </c>
-      <c r="H98" s="8" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="66"/>
-      <c r="G99" s="68"/>
-      <c r="H99" s="8"/>
-    </row>
-    <row r="100" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="70"/>
-      <c r="B100" s="71" t="s">
-        <v>172</v>
-      </c>
-      <c r="C100" s="71" t="s">
-        <v>173</v>
-      </c>
-      <c r="D100" s="71"/>
-      <c r="E100" s="71"/>
-      <c r="F100" s="71"/>
-      <c r="G100" s="72"/>
-      <c r="H100" s="73"/>
-    </row>
-    <row r="101" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="62"/>
-      <c r="B101" s="63"/>
-      <c r="C101" s="74" t="s">
-        <v>174</v>
-      </c>
-      <c r="D101" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E101" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F101" s="63"/>
-      <c r="G101" s="64" t="n">
-        <v>1</v>
-      </c>
-      <c r="H101" s="65" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="66"/>
-      <c r="C102" s="74"/>
-      <c r="D102" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="E102" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="G102" s="68" t="s">
-        <v>100</v>
-      </c>
-      <c r="H102" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="66"/>
-      <c r="C103" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="D103" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="E103" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="G103" s="68" t="s">
-        <v>156</v>
-      </c>
-      <c r="H103" s="8" t="n">
+      <c r="H105" s="8" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="75"/>
-      <c r="B104" s="76"/>
-      <c r="C104" s="76"/>
-      <c r="D104" s="76"/>
-      <c r="E104" s="76"/>
-      <c r="F104" s="76"/>
-      <c r="G104" s="77"/>
-      <c r="H104" s="78"/>
+    <row r="106" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="75"/>
+      <c r="B106" s="76"/>
+      <c r="C106" s="76"/>
+      <c r="D106" s="76"/>
+      <c r="E106" s="76"/>
+      <c r="F106" s="76"/>
+      <c r="G106" s="77"/>
+      <c r="H106" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -3075,11 +3091,11 @@
     <mergeCell ref="C50:C51"/>
     <mergeCell ref="C57:C58"/>
     <mergeCell ref="C71:C72"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="C89:C91"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="C101:C102"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C95:C96"/>
+    <mergeCell ref="C98:C100"/>
+    <mergeCell ref="C103:C104"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Eliminate annoying periodic "Stabilized Flight Mode" announcements.
v2.50 2020-01-12 AutoAP: Activate udp broadcast on AP dhcp allocated IP subnet.
                 Eliminate annoying periodic "Stabilized Flight Mode" announcements.
                 Further localise options in to logical groups.
</commit_message>
<xml_diff>
--- a/Mavlink_Frsky_Passthru_Telemetry_Extended.xlsx
+++ b/Mavlink_Frsky_Passthru_Telemetry_Extended.xlsx
@@ -406,7 +406,7 @@
     <t xml:space="preserve">number</t>
   </si>
   <si>
-    <t xml:space="preserve">ParamId   1,2,3,4....</t>
+    <t xml:space="preserve">Param-Id   1,2,3,4....</t>
   </si>
   <si>
     <t xml:space="preserve">25-28</t>
@@ -1176,8 +1176,8 @@
   </sheetPr>
   <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A63" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B104" activeCellId="0" sqref="B104"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C67" activeCellId="0" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2307,7 +2307,9 @@
         <v>8</v>
       </c>
       <c r="G61" s="53"/>
-      <c r="H61" s="33"/>
+      <c r="H61" s="33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="46"/>
@@ -2323,7 +2325,9 @@
       </c>
       <c r="F62" s="36"/>
       <c r="G62" s="58"/>
-      <c r="H62" s="57"/>
+      <c r="H62" s="57" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="46"/>

</xml_diff>

<commit_message>
v2.29.2 2020-04-21 Some structural tidying up.
v2.29.2 2020-04-21 Some structural tidying up.
</commit_message>
<xml_diff>
--- a/Mavlink_Frsky_Passthru_Telemetry_Extended.xlsx
+++ b/Mavlink_Frsky_Passthru_Telemetry_Extended.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="179">
   <si>
     <t xml:space="preserve">Source</t>
   </si>
@@ -316,19 +316,25 @@
     <t xml:space="preserve">#74</t>
   </si>
   <si>
+    <t xml:space="preserve">hud vx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decimeters/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hud vy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horizontal velocity / groundspeed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-16</t>
+  </si>
+  <si>
     <t xml:space="preserve">hud</t>
-  </si>
-  <si>
-    <t xml:space="preserve">decimeters/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Horizontal velocity / groundspeed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11-16</t>
   </si>
   <si>
     <t xml:space="preserve">Yaw / Heading</t>
@@ -1176,8 +1182,8 @@
   </sheetPr>
   <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C67" activeCellId="0" sqref="C67"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C47" activeCellId="0" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2091,10 +2097,10 @@
         <v>97</v>
       </c>
       <c r="B50" s="30" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C50" s="45" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D50" s="17" t="s">
         <v>57</v>
@@ -2122,7 +2128,7 @@
       </c>
       <c r="F51" s="32"/>
       <c r="G51" s="23" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H51" s="33" t="n">
         <v>10</v>
@@ -2133,20 +2139,20 @@
         <v>97</v>
       </c>
       <c r="B52" s="30" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D52" s="32" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E52" s="32" t="n">
         <v>11</v>
       </c>
       <c r="F52" s="32"/>
       <c r="G52" s="23" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H52" s="33" t="n">
         <v>16</v>
@@ -2166,10 +2172,10 @@
     <row r="54" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="24"/>
       <c r="B54" s="25" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C54" s="26" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D54" s="26"/>
       <c r="E54" s="26"/>
@@ -2183,19 +2189,19 @@
       <c r="A55" s="29"/>
       <c r="B55" s="30"/>
       <c r="C55" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D55" s="32" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E55" s="32" t="n">
         <v>11</v>
       </c>
       <c r="F55" s="32" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G55" s="23" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H55" s="33" t="n">
         <v>0</v>
@@ -2205,19 +2211,19 @@
       <c r="A56" s="29"/>
       <c r="B56" s="30"/>
       <c r="C56" s="32" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D56" s="32" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E56" s="32" t="n">
         <v>10</v>
       </c>
       <c r="F56" s="32" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G56" s="23" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H56" s="33" t="n">
         <v>11</v>
@@ -2227,7 +2233,7 @@
       <c r="A57" s="29"/>
       <c r="B57" s="30"/>
       <c r="C57" s="45" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D57" s="17" t="s">
         <v>57</v>
@@ -2248,13 +2254,13 @@
       <c r="B58" s="30"/>
       <c r="C58" s="45"/>
       <c r="D58" s="32" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E58" s="32" t="n">
         <v>10</v>
       </c>
       <c r="G58" s="23" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H58" s="33" t="n">
         <v>22</v>
@@ -2277,10 +2283,10 @@
     <row r="60" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="24"/>
       <c r="B60" s="25" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C60" s="26" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D60" s="26" t="s">
         <v>22</v>
@@ -2289,7 +2295,7 @@
         <v>8</v>
       </c>
       <c r="F60" s="26" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G60" s="27"/>
       <c r="H60" s="28"/>
@@ -2298,7 +2304,7 @@
       <c r="A61" s="29"/>
       <c r="B61" s="35"/>
       <c r="C61" s="22" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D61" s="36" t="s">
         <v>22</v>
@@ -2315,7 +2321,7 @@
       <c r="A62" s="46"/>
       <c r="B62" s="47"/>
       <c r="C62" s="17" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D62" s="17" t="s">
         <v>79</v>
@@ -2333,7 +2339,7 @@
       <c r="A63" s="46"/>
       <c r="B63" s="47"/>
       <c r="C63" s="17" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D63" s="17" t="s">
         <v>79</v>
@@ -2349,10 +2355,10 @@
       <c r="A64" s="46"/>
       <c r="B64" s="59"/>
       <c r="C64" s="22" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D64" s="36" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E64" s="22" t="n">
         <v>24</v>
@@ -2365,7 +2371,7 @@
       <c r="A65" s="29"/>
       <c r="B65" s="30"/>
       <c r="C65" s="22" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D65" s="17" t="s">
         <v>79</v>
@@ -2381,10 +2387,10 @@
       <c r="A66" s="29"/>
       <c r="B66" s="30"/>
       <c r="C66" s="22" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D66" s="17" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E66" s="17" t="n">
         <v>24</v>
@@ -2397,7 +2403,7 @@
       <c r="A67" s="29"/>
       <c r="B67" s="30"/>
       <c r="C67" s="32" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D67" s="32"/>
       <c r="E67" s="32" t="n">
@@ -2405,7 +2411,7 @@
       </c>
       <c r="F67" s="32"/>
       <c r="G67" s="23" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H67" s="33" t="n">
         <v>24</v>
@@ -2426,10 +2432,10 @@
     <row r="69" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="24"/>
       <c r="B69" s="25" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C69" s="26" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D69" s="26"/>
       <c r="E69" s="26"/>
@@ -2535,10 +2541,10 @@
     <row r="75" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="61"/>
       <c r="B75" s="26" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C75" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D75" s="26"/>
       <c r="E75" s="26"/>
@@ -2551,7 +2557,7 @@
     <row r="76" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="62"/>
       <c r="C76" s="63" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D76" s="63"/>
       <c r="E76" s="63" t="n">
@@ -2559,7 +2565,7 @@
       </c>
       <c r="F76" s="63"/>
       <c r="G76" s="64" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H76" s="65" t="n">
         <v>0</v>
@@ -2568,7 +2574,7 @@
     <row r="77" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="66"/>
       <c r="C77" s="67" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D77" s="0" t="s">
         <v>57</v>
@@ -2587,13 +2593,13 @@
       <c r="A78" s="66"/>
       <c r="C78" s="67"/>
       <c r="D78" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E78" s="0" t="n">
         <v>10</v>
       </c>
       <c r="G78" s="68" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H78" s="8" t="n">
         <v>12</v>
@@ -2602,7 +2608,7 @@
     <row r="79" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="66"/>
       <c r="C79" s="67" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D79" s="0" t="s">
         <v>57</v>
@@ -2621,13 +2627,13 @@
       <c r="A80" s="66"/>
       <c r="C80" s="67"/>
       <c r="D80" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E80" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G80" s="68" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H80" s="8" t="n">
         <v>23</v>
@@ -2636,16 +2642,16 @@
     <row r="81" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="66"/>
       <c r="C81" s="69" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E81" s="0" t="n">
         <v>3</v>
       </c>
       <c r="G81" s="68" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H81" s="8" t="n">
         <v>29</v>
@@ -2659,13 +2665,13 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="24" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B83" s="25" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C83" s="26" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D83" s="26"/>
       <c r="E83" s="26"/>
@@ -2679,14 +2685,14 @@
       <c r="A84" s="29"/>
       <c r="B84" s="30"/>
       <c r="C84" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D84" s="32"/>
       <c r="E84" s="32" t="n">
         <v>4</v>
       </c>
       <c r="F84" s="32" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="G84" s="23" t="s">
         <v>52</v>
@@ -2699,17 +2705,17 @@
       <c r="A85" s="29"/>
       <c r="B85" s="30"/>
       <c r="C85" s="32" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D85" s="32"/>
       <c r="E85" s="32" t="n">
         <v>6</v>
       </c>
       <c r="F85" s="32" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G85" s="23" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H85" s="33" t="n">
         <v>4</v>
@@ -2719,14 +2725,14 @@
       <c r="A86" s="29"/>
       <c r="B86" s="30"/>
       <c r="C86" s="32" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D86" s="32"/>
       <c r="E86" s="32" t="n">
         <v>1</v>
       </c>
       <c r="F86" s="32" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G86" s="23" t="n">
         <v>11</v>
@@ -2739,17 +2745,17 @@
       <c r="A87" s="29"/>
       <c r="B87" s="30"/>
       <c r="C87" s="32" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D87" s="32"/>
       <c r="E87" s="32" t="n">
         <v>6</v>
       </c>
       <c r="F87" s="32" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G87" s="23" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H87" s="33" t="n">
         <v>11</v>
@@ -2759,14 +2765,14 @@
       <c r="A88" s="29"/>
       <c r="B88" s="30"/>
       <c r="C88" s="32" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D88" s="32"/>
       <c r="E88" s="32" t="n">
         <v>1</v>
       </c>
       <c r="F88" s="32" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G88" s="23" t="n">
         <v>18</v>
@@ -2779,17 +2785,17 @@
       <c r="A89" s="29"/>
       <c r="B89" s="30"/>
       <c r="C89" s="32" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D89" s="32"/>
       <c r="E89" s="32" t="n">
         <v>6</v>
       </c>
       <c r="F89" s="32" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G89" s="23" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H89" s="33" t="n">
         <v>18</v>
@@ -2799,14 +2805,14 @@
       <c r="A90" s="29"/>
       <c r="B90" s="30"/>
       <c r="C90" s="32" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D90" s="32"/>
       <c r="E90" s="32" t="n">
         <v>1</v>
       </c>
       <c r="F90" s="32" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G90" s="23" t="n">
         <v>25</v>
@@ -2819,17 +2825,17 @@
       <c r="A91" s="29"/>
       <c r="B91" s="30"/>
       <c r="C91" s="32" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D91" s="32"/>
       <c r="E91" s="32" t="n">
         <v>6</v>
       </c>
       <c r="F91" s="32" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G91" s="23" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H91" s="33" t="n">
         <v>25</v>
@@ -2839,14 +2845,14 @@
       <c r="A92" s="29"/>
       <c r="B92" s="30"/>
       <c r="C92" s="32" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D92" s="32"/>
       <c r="E92" s="32" t="n">
         <v>1</v>
       </c>
       <c r="F92" s="32" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G92" s="23" t="n">
         <v>32</v>
@@ -2870,10 +2876,10 @@
         <v>97</v>
       </c>
       <c r="B94" s="25" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C94" s="26" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D94" s="26"/>
       <c r="E94" s="26"/>
@@ -2889,7 +2895,7 @@
       <c r="A95" s="29"/>
       <c r="B95" s="30"/>
       <c r="C95" s="45" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D95" s="17" t="s">
         <v>57</v>
@@ -2927,17 +2933,17 @@
       <c r="A97" s="29"/>
       <c r="B97" s="30"/>
       <c r="C97" s="32" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D97" s="32"/>
       <c r="E97" s="32" t="n">
         <v>7</v>
       </c>
       <c r="F97" s="32" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G97" s="23" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H97" s="33" t="n">
         <v>8</v>
@@ -2947,7 +2953,7 @@
       <c r="A98" s="29"/>
       <c r="B98" s="30"/>
       <c r="C98" s="45" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D98" s="17" t="s">
         <v>57</v>
@@ -2957,7 +2963,7 @@
       </c>
       <c r="F98" s="32"/>
       <c r="G98" s="23" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H98" s="33" t="n">
         <v>15</v>
@@ -2975,7 +2981,7 @@
       </c>
       <c r="F99" s="32"/>
       <c r="G99" s="23" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="H99" s="33" t="n">
         <v>17</v>
@@ -3007,10 +3013,10 @@
     <row r="102" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="70"/>
       <c r="B102" s="71" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C102" s="71" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D102" s="71"/>
       <c r="E102" s="71"/>
@@ -3022,7 +3028,7 @@
       <c r="A103" s="62"/>
       <c r="B103" s="63"/>
       <c r="C103" s="74" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D103" s="0" t="s">
         <v>57</v>
@@ -3042,7 +3048,7 @@
       <c r="A104" s="66"/>
       <c r="C104" s="74"/>
       <c r="D104" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E104" s="0" t="n">
         <v>7</v>
@@ -3057,7 +3063,7 @@
     <row r="105" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="66"/>
       <c r="C105" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D105" s="0" t="s">
         <v>92</v>
@@ -3066,7 +3072,7 @@
         <v>7</v>
       </c>
       <c r="G105" s="68" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H105" s="8" t="n">
         <v>8</v>

</xml_diff>

<commit_message>
Added ILI9341 2.8" 320 x 240 colour, basic HUD
v2.63.5 2020-12-04  Support added for ILI9341 2.8" 320 x 240 colour display
                    Simple HUD for flight info display. Needs more work.
</commit_message>
<xml_diff>
--- a/Mavlink_Frsky_Passthru_Telemetry_Extended.xlsx
+++ b/Mavlink_Frsky_Passthru_Telemetry_Extended.xlsx
@@ -304,7 +304,7 @@
     <t xml:space="preserve">26-32</t>
   </si>
   <si>
-    <t xml:space="preserve">0x005</t>
+    <t xml:space="preserve">0x5005</t>
   </si>
   <si>
     <t xml:space="preserve">VELANDYAW (2Hz)</t>
@@ -1176,25 +1176,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H106"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C47" activeCellId="0" sqref="C47"/>
+      <selection pane="topLeft" activeCell="B46" activeCellId="0" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.47"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.18"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.26"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
A few small improvements
</commit_message>
<xml_diff>
--- a/Mavlink_Frsky_Passthru_Telemetry_Extended.xlsx
+++ b/Mavlink_Frsky_Passthru_Telemetry_Extended.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/da4e155d334c076a/Documents/GitHub/MavlinkToPassthru/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_D806B4535B162FC63FCEA2D7413B2F0BE852CC3E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45A65F91-9CAA-42CA-ABC9-5065B2E89CF8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -561,7 +567,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000"/>
   </numFmts>
@@ -803,30 +809,6 @@
   </cellStyleXfs>
   <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -965,6 +947,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1043,6 +1049,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1090,7 +1099,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1123,9 +1132,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1158,6 +1184,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1333,10 +1376,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
@@ -1346,1386 +1389,1386 @@
     <col min="3" max="3" width="44.140625" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="6.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="88.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9" t="s">
+      <c r="G1" s="1"/>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="16"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="11">
         <v>30</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="22"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="25" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25">
+      <c r="D4" s="17"/>
+      <c r="E4" s="17">
         <v>2</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H4" s="20">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="31" t="s">
+      <c r="A5" s="15"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="28"/>
+      <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="33" t="s">
+      <c r="A6" s="24"/>
+      <c r="B6" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34">
+      <c r="D6" s="26"/>
+      <c r="E6" s="26">
         <v>32</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="35"/>
-      <c r="H6" s="36"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="28"/>
     </row>
     <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="39" t="s">
+      <c r="A7" s="29"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="40">
+      <c r="E7" s="32">
         <v>3</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="31"/>
-      <c r="H7" s="41"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="33"/>
     </row>
     <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="42" t="s">
+      <c r="A8" s="29"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="40">
+      <c r="E8" s="32">
         <v>32</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="F8" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="31" t="s">
+      <c r="G8" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="41"/>
+      <c r="H8" s="33"/>
     </row>
     <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="G9" s="31" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="G9" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="28"/>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="33" t="s">
+      <c r="A10" s="24"/>
+      <c r="B10" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="36" t="s">
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="28" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="40" t="s">
+      <c r="A11" s="29"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D11" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="40">
+      <c r="E11" s="32">
         <v>5</v>
       </c>
-      <c r="F11" s="40" t="s">
+      <c r="F11" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="41">
+      <c r="H11" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="40" t="s">
+      <c r="A12" s="29"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="40">
+      <c r="E12" s="32">
         <v>2</v>
       </c>
-      <c r="F12" s="40"/>
-      <c r="G12" s="31" t="s">
+      <c r="F12" s="32"/>
+      <c r="G12" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="41">
+      <c r="H12" s="33">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="40" t="s">
+      <c r="A13" s="29"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="40">
+      <c r="E13" s="32">
         <v>1</v>
       </c>
-      <c r="F13" s="40"/>
-      <c r="G13" s="31">
+      <c r="F13" s="32"/>
+      <c r="G13" s="23">
         <v>8</v>
       </c>
-      <c r="H13" s="41">
+      <c r="H13" s="33">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="40" t="s">
+      <c r="A14" s="29"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="40" t="s">
+      <c r="D14" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="40">
+      <c r="E14" s="32">
         <v>1</v>
       </c>
-      <c r="F14" s="40"/>
-      <c r="G14" s="31">
+      <c r="F14" s="32"/>
+      <c r="G14" s="23">
         <v>9</v>
       </c>
-      <c r="H14" s="41">
+      <c r="H14" s="33">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="37"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="40" t="s">
+      <c r="A15" s="29"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="40">
+      <c r="E15" s="32">
         <v>1</v>
       </c>
-      <c r="F15" s="40"/>
-      <c r="G15" s="31">
+      <c r="F15" s="32"/>
+      <c r="G15" s="23">
         <v>10</v>
       </c>
-      <c r="H15" s="41">
+      <c r="H15" s="33">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="25" t="s">
+      <c r="A16" s="15"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="17">
         <v>2</v>
       </c>
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="28">
+      <c r="H16" s="20">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="25" t="s">
+      <c r="A17" s="15"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25">
+      <c r="D17" s="17"/>
+      <c r="E17" s="17">
         <v>1</v>
       </c>
       <c r="F17" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="19">
         <v>13</v>
       </c>
-      <c r="H17" s="28">
+      <c r="H17" s="20">
         <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="25" t="s">
+      <c r="A18" s="15"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25">
+      <c r="D18" s="17"/>
+      <c r="E18" s="17">
         <v>13</v>
       </c>
-      <c r="G18" s="27" t="s">
+      <c r="G18" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="H18" s="28">
+      <c r="H18" s="20">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="25" t="s">
+      <c r="A19" s="15"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25">
+      <c r="D19" s="17"/>
+      <c r="E19" s="17">
         <v>6</v>
       </c>
-      <c r="G19" s="27" t="s">
+      <c r="G19" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="H19" s="28">
+      <c r="H19" s="20">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="37"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="40" t="s">
+      <c r="A20" s="29"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="31" t="s">
+      <c r="G20" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="41"/>
+      <c r="H20" s="33"/>
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
-      <c r="B21" s="33" t="s">
+      <c r="A21" s="24"/>
+      <c r="B21" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="45" t="s">
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="37" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="37"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="40" t="s">
+      <c r="A22" s="29"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="40">
+      <c r="E22" s="32">
         <v>4</v>
       </c>
-      <c r="F22" s="40" t="s">
+      <c r="F22" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="31" t="s">
+      <c r="G22" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="H22" s="41"/>
+      <c r="H22" s="33"/>
     </row>
     <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="37"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="40" t="s">
+      <c r="A23" s="29"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="40" t="s">
+      <c r="D23" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="40">
+      <c r="E23" s="32">
         <v>2</v>
       </c>
-      <c r="F23" s="40" t="s">
+      <c r="F23" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="G23" s="31" t="s">
+      <c r="G23" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="H23" s="41">
+      <c r="H23" s="33">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="37"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="8" t="s">
+      <c r="A24" s="29"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="76" t="s">
         <v>56</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D24" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="17">
         <v>1</v>
       </c>
-      <c r="F24" s="40"/>
-      <c r="G24" s="31">
+      <c r="F24" s="32"/>
+      <c r="G24" s="23">
         <v>7</v>
       </c>
-      <c r="H24" s="41">
+      <c r="H24" s="33">
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="37"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="25" t="s">
+      <c r="A25" s="29"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="17">
         <v>7</v>
       </c>
-      <c r="F25" s="40" t="s">
+      <c r="F25" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="G25" s="31" t="s">
+      <c r="G25" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="H25" s="41">
+      <c r="H25" s="33">
         <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="8" t="s">
+      <c r="A26" s="15"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="46">
+      <c r="E26" s="38">
         <v>2</v>
       </c>
-      <c r="F26" s="25" t="s">
+      <c r="F26" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="G26" s="47" t="s">
+      <c r="G26" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="H26" s="48">
+      <c r="H26" s="40">
         <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="40" t="s">
+      <c r="A27" s="15"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="76"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="G27" s="49" t="s">
+      <c r="G27" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="H27" s="28">
+      <c r="H27" s="20">
         <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="6" t="s">
+      <c r="A28" s="15"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="78" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="25" t="s">
+      <c r="D28" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E28" s="25">
+      <c r="E28" s="17">
         <v>2</v>
       </c>
-      <c r="F28" s="40"/>
-      <c r="G28" s="27" t="s">
+      <c r="F28" s="32"/>
+      <c r="G28" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="H28" s="28">
+      <c r="H28" s="20">
         <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="25" t="s">
+      <c r="A29" s="15"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="78"/>
+      <c r="D29" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="17">
         <v>7</v>
       </c>
-      <c r="F29" s="40"/>
-      <c r="G29" s="27" t="s">
+      <c r="F29" s="32"/>
+      <c r="G29" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="H29" s="28">
+      <c r="H29" s="20">
         <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="40" t="s">
+      <c r="A30" s="15"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="78"/>
+      <c r="D30" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="E30" s="40">
+      <c r="E30" s="32">
         <v>1</v>
       </c>
-      <c r="F30" s="25"/>
-      <c r="G30" s="27">
+      <c r="F30" s="17"/>
+      <c r="G30" s="19">
         <v>32</v>
       </c>
-      <c r="H30" s="28">
+      <c r="H30" s="20">
         <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="37"/>
-      <c r="B31" s="38"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="G31" s="31" t="s">
+      <c r="A31" s="29"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="G31" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H31" s="41"/>
+      <c r="H31" s="33"/>
     </row>
     <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
-      <c r="B32" s="33" t="s">
+      <c r="A32" s="24"/>
+      <c r="B32" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="36"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="28"/>
     </row>
     <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="37"/>
-      <c r="B33" s="38"/>
-      <c r="C33" s="40" t="s">
+      <c r="A33" s="29"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="40" t="s">
+      <c r="D33" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="E33" s="40">
+      <c r="E33" s="32">
         <v>9</v>
       </c>
-      <c r="F33" s="40" t="s">
+      <c r="F33" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="G33" s="31" t="s">
+      <c r="G33" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="H33" s="41">
+      <c r="H33" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="37"/>
-      <c r="B34" s="38"/>
-      <c r="C34" s="5" t="s">
+      <c r="A34" s="29"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="72" t="s">
         <v>75</v>
       </c>
-      <c r="D34" s="25" t="s">
+      <c r="D34" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="25">
+      <c r="E34" s="17">
         <v>1</v>
       </c>
-      <c r="F34" s="40"/>
-      <c r="G34" s="31">
+      <c r="F34" s="32"/>
+      <c r="G34" s="23">
         <v>10</v>
       </c>
-      <c r="H34" s="41">
+      <c r="H34" s="33">
         <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="37"/>
-      <c r="B35" s="38"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="40" t="s">
+      <c r="A35" s="29"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E35" s="17">
         <v>7</v>
       </c>
-      <c r="F35" s="40"/>
-      <c r="G35" s="31" t="s">
+      <c r="F35" s="32"/>
+      <c r="G35" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="H35" s="41">
+      <c r="H35" s="33">
         <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="50"/>
-      <c r="B36" s="51"/>
-      <c r="C36" s="25" t="s">
+      <c r="A36" s="42"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="25" t="s">
+      <c r="D36" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E36" s="25">
+      <c r="E36" s="17">
         <v>15</v>
       </c>
-      <c r="F36" s="25" t="s">
+      <c r="F36" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="G36" s="31" t="s">
+      <c r="G36" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="H36" s="41">
+      <c r="H36" s="33">
         <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="37"/>
-      <c r="B37" s="38"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="40"/>
-      <c r="G37" s="31" t="s">
+      <c r="A37" s="29"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+      <c r="G37" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H37" s="41"/>
+      <c r="H37" s="33"/>
     </row>
     <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="32"/>
-      <c r="B38" s="33" t="s">
+      <c r="A38" s="24"/>
+      <c r="B38" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="C38" s="34" t="s">
+      <c r="C38" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="35"/>
-      <c r="H38" s="45" t="s">
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="37" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="37"/>
-      <c r="B39" s="38"/>
-      <c r="C39" s="4" t="s">
+      <c r="A39" s="29"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="74" t="s">
         <v>84</v>
       </c>
-      <c r="D39" s="25" t="s">
+      <c r="D39" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E39" s="40">
+      <c r="E39" s="32">
         <v>2</v>
       </c>
-      <c r="F39" s="40" t="s">
+      <c r="F39" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="G39" s="31" t="s">
+      <c r="G39" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="H39" s="41">
+      <c r="H39" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="37"/>
-      <c r="B40" s="38"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="40" t="s">
+      <c r="A40" s="29"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="74"/>
+      <c r="D40" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="E40" s="40">
+      <c r="E40" s="32">
         <v>10</v>
       </c>
-      <c r="F40" s="40"/>
-      <c r="G40" s="31" t="s">
+      <c r="F40" s="32"/>
+      <c r="G40" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="H40" s="41">
+      <c r="H40" s="33">
         <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="37"/>
-      <c r="B41" s="38"/>
-      <c r="C41" s="3" t="s">
+      <c r="A41" s="29"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="D41" s="25" t="s">
+      <c r="D41" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="52">
+      <c r="E41" s="44">
         <v>2</v>
       </c>
-      <c r="F41" s="40"/>
-      <c r="G41" s="53" t="s">
+      <c r="F41" s="32"/>
+      <c r="G41" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="H41" s="41">
+      <c r="H41" s="33">
         <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="37"/>
-      <c r="B42" s="38"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="40" t="s">
+      <c r="A42" s="29"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="75"/>
+      <c r="D42" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="E42" s="52">
+      <c r="E42" s="44">
         <v>10</v>
       </c>
-      <c r="F42" s="40"/>
-      <c r="G42" s="53" t="s">
+      <c r="F42" s="32"/>
+      <c r="G42" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="H42" s="41">
+      <c r="H42" s="33">
         <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="37"/>
-      <c r="B43" s="38"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="40" t="s">
+      <c r="A43" s="29"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="75"/>
+      <c r="D43" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="E43" s="52">
+      <c r="E43" s="44">
         <v>1</v>
       </c>
-      <c r="F43" s="54"/>
-      <c r="G43" s="53">
+      <c r="F43" s="46"/>
+      <c r="G43" s="45">
         <v>25</v>
       </c>
-      <c r="H43" s="41">
+      <c r="H43" s="33">
         <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="37"/>
-      <c r="B44" s="38"/>
-      <c r="C44" s="40" t="s">
+      <c r="A44" s="29"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="D44" s="40" t="s">
+      <c r="D44" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="E44" s="40">
+      <c r="E44" s="32">
         <v>7</v>
       </c>
-      <c r="F44" s="40"/>
-      <c r="G44" s="31" t="s">
+      <c r="F44" s="32"/>
+      <c r="G44" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="H44" s="41">
+      <c r="H44" s="33">
         <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="37"/>
-      <c r="B45" s="38"/>
-      <c r="C45" s="40"/>
-      <c r="D45" s="40"/>
-      <c r="E45" s="40"/>
-      <c r="G45" s="31" t="s">
+      <c r="A45" s="29"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+      <c r="G45" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H45" s="41"/>
+      <c r="H45" s="33"/>
     </row>
     <row r="46" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="32"/>
-      <c r="B46" s="33" t="s">
+      <c r="A46" s="24"/>
+      <c r="B46" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="C46" s="34" t="s">
+      <c r="C46" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="D46" s="34"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="35"/>
-      <c r="H46" s="45" t="s">
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="37" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="37"/>
-      <c r="B47" s="43"/>
-      <c r="C47" s="4" t="s">
+      <c r="A47" s="29"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="74" t="s">
         <v>96</v>
       </c>
-      <c r="D47" s="25" t="s">
+      <c r="D47" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E47" s="44">
+      <c r="E47" s="36">
         <v>1</v>
       </c>
-      <c r="F47" s="40" t="s">
+      <c r="F47" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="G47" s="55">
+      <c r="G47" s="47">
         <v>1</v>
       </c>
-      <c r="H47" s="41">
+      <c r="H47" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="37" t="s">
+      <c r="A48" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="B48" s="38" t="s">
+      <c r="B48" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="40" t="s">
+      <c r="C48" s="74"/>
+      <c r="D48" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="E48" s="40">
+      <c r="E48" s="32">
         <v>7</v>
       </c>
-      <c r="F48" s="40"/>
-      <c r="G48" s="31" t="s">
+      <c r="F48" s="32"/>
+      <c r="G48" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="H48" s="41">
+      <c r="H48" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="37"/>
-      <c r="B49" s="38"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="40" t="s">
+      <c r="A49" s="29"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="74"/>
+      <c r="D49" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="E49" s="40">
+      <c r="E49" s="32">
         <v>1</v>
       </c>
-      <c r="F49" s="56"/>
-      <c r="G49" s="31">
+      <c r="F49" s="48"/>
+      <c r="G49" s="23">
         <v>9</v>
       </c>
-      <c r="H49" s="41">
+      <c r="H49" s="33">
         <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="37" t="s">
+      <c r="A50" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="B50" s="38" t="s">
+      <c r="B50" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="D50" s="25" t="s">
+      <c r="D50" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E50" s="40">
+      <c r="E50" s="32">
         <v>1</v>
       </c>
-      <c r="F50" s="40"/>
-      <c r="G50" s="31">
+      <c r="F50" s="32"/>
+      <c r="G50" s="23">
         <v>10</v>
       </c>
-      <c r="H50" s="41">
+      <c r="H50" s="33">
         <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="37"/>
-      <c r="B51" s="38"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="40" t="s">
+      <c r="A51" s="29"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="72"/>
+      <c r="D51" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="E51" s="40">
+      <c r="E51" s="32">
         <v>7</v>
       </c>
-      <c r="F51" s="40"/>
-      <c r="G51" s="31" t="s">
+      <c r="F51" s="32"/>
+      <c r="G51" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="H51" s="41">
+      <c r="H51" s="33">
         <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="37" t="s">
+      <c r="A52" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="B52" s="38" t="s">
+      <c r="B52" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="C52" s="40" t="s">
+      <c r="C52" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="D52" s="40" t="s">
+      <c r="D52" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="E52" s="40">
+      <c r="E52" s="32">
         <v>11</v>
       </c>
-      <c r="F52" s="40"/>
-      <c r="G52" s="31" t="s">
+      <c r="F52" s="32"/>
+      <c r="G52" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="H52" s="41">
+      <c r="H52" s="33">
         <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="50"/>
-      <c r="B53" s="51"/>
-      <c r="C53" s="57"/>
-      <c r="D53" s="58"/>
-      <c r="E53" s="58"/>
-      <c r="G53" s="31" t="s">
+      <c r="A53" s="42"/>
+      <c r="B53" s="43"/>
+      <c r="C53" s="49"/>
+      <c r="D53" s="50"/>
+      <c r="E53" s="50"/>
+      <c r="G53" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H53" s="59"/>
+      <c r="H53" s="51"/>
     </row>
     <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="32"/>
-      <c r="B54" s="33" t="s">
+      <c r="A54" s="24"/>
+      <c r="B54" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="C54" s="34" t="s">
+      <c r="C54" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="D54" s="34"/>
-      <c r="E54" s="34"/>
-      <c r="F54" s="34"/>
-      <c r="G54" s="35"/>
-      <c r="H54" s="45" t="s">
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="27"/>
+      <c r="H54" s="37" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="37"/>
-      <c r="B55" s="38"/>
-      <c r="C55" s="40" t="s">
+      <c r="A55" s="29"/>
+      <c r="B55" s="30"/>
+      <c r="C55" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="D55" s="40" t="s">
+      <c r="D55" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="E55" s="40">
+      <c r="E55" s="32">
         <v>11</v>
       </c>
-      <c r="F55" s="40" t="s">
+      <c r="F55" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="G55" s="31" t="s">
+      <c r="G55" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="H55" s="41">
+      <c r="H55" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="37"/>
-      <c r="B56" s="38"/>
-      <c r="C56" s="40" t="s">
+      <c r="A56" s="29"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="D56" s="40" t="s">
+      <c r="D56" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="E56" s="40">
+      <c r="E56" s="32">
         <v>10</v>
       </c>
-      <c r="F56" s="40" t="s">
+      <c r="F56" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="G56" s="31" t="s">
+      <c r="G56" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="H56" s="41">
+      <c r="H56" s="33">
         <v>11</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="37"/>
-      <c r="B57" s="38"/>
-      <c r="C57" s="5" t="s">
+      <c r="A57" s="29"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="72" t="s">
         <v>116</v>
       </c>
-      <c r="D57" s="25" t="s">
+      <c r="D57" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E57" s="40">
+      <c r="E57" s="32">
         <v>1</v>
       </c>
-      <c r="F57" s="40"/>
-      <c r="G57" s="31">
+      <c r="F57" s="32"/>
+      <c r="G57" s="23">
         <v>22</v>
       </c>
-      <c r="H57" s="41">
+      <c r="H57" s="33">
         <v>21</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="37"/>
-      <c r="B58" s="38"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="40" t="s">
+      <c r="A58" s="29"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="72"/>
+      <c r="D58" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="E58" s="40">
+      <c r="E58" s="32">
         <v>10</v>
       </c>
-      <c r="G58" s="31" t="s">
+      <c r="G58" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="H58" s="41">
+      <c r="H58" s="33">
         <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="37"/>
-      <c r="B59" s="38"/>
-      <c r="C59" s="54"/>
-      <c r="D59" s="40"/>
-      <c r="E59" s="54"/>
-      <c r="F59" s="40" t="s">
+      <c r="A59" s="29"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="46"/>
+      <c r="D59" s="32"/>
+      <c r="E59" s="46"/>
+      <c r="F59" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="G59" s="31" t="s">
+      <c r="G59" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H59" s="41"/>
+      <c r="H59" s="33"/>
     </row>
     <row r="60" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="32"/>
-      <c r="B60" s="33" t="s">
+      <c r="A60" s="24"/>
+      <c r="B60" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="C60" s="34" t="s">
+      <c r="C60" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="D60" s="34" t="s">
+      <c r="D60" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="E60" s="34">
+      <c r="E60" s="26">
         <v>8</v>
       </c>
-      <c r="F60" s="34" t="s">
+      <c r="F60" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="G60" s="35"/>
-      <c r="H60" s="36"/>
+      <c r="G60" s="27"/>
+      <c r="H60" s="28"/>
     </row>
     <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="37"/>
-      <c r="B61" s="43"/>
-      <c r="C61" s="30" t="s">
+      <c r="A61" s="29"/>
+      <c r="B61" s="35"/>
+      <c r="C61" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="D61" s="44" t="s">
+      <c r="D61" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="E61" s="44">
+      <c r="E61" s="36">
         <v>8</v>
       </c>
-      <c r="G61" s="55"/>
-      <c r="H61" s="41">
+      <c r="G61" s="47"/>
+      <c r="H61" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="50"/>
-      <c r="B62" s="51"/>
-      <c r="C62" s="25" t="s">
+      <c r="A62" s="42"/>
+      <c r="B62" s="43"/>
+      <c r="C62" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D62" s="25" t="s">
+      <c r="D62" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E62" s="25">
+      <c r="E62" s="17">
         <v>24</v>
       </c>
-      <c r="F62" s="44"/>
-      <c r="G62" s="60"/>
-      <c r="H62" s="59">
+      <c r="F62" s="36"/>
+      <c r="G62" s="52"/>
+      <c r="H62" s="51">
         <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="50"/>
-      <c r="B63" s="51"/>
-      <c r="C63" s="25" t="s">
+      <c r="A63" s="42"/>
+      <c r="B63" s="43"/>
+      <c r="C63" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="D63" s="25" t="s">
+      <c r="D63" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E63" s="25">
+      <c r="E63" s="17">
         <v>24</v>
       </c>
-      <c r="F63" s="44"/>
-      <c r="G63" s="60"/>
-      <c r="H63" s="59"/>
+      <c r="F63" s="36"/>
+      <c r="G63" s="52"/>
+      <c r="H63" s="51"/>
     </row>
     <row r="64" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="50"/>
-      <c r="B64" s="61"/>
-      <c r="C64" s="30" t="s">
+      <c r="A64" s="42"/>
+      <c r="B64" s="53"/>
+      <c r="C64" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="D64" s="44" t="s">
+      <c r="D64" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="E64" s="30">
+      <c r="E64" s="22">
         <v>24</v>
       </c>
-      <c r="F64" s="40"/>
-      <c r="G64" s="62"/>
-      <c r="H64" s="59"/>
+      <c r="F64" s="32"/>
+      <c r="G64" s="54"/>
+      <c r="H64" s="51"/>
     </row>
     <row r="65" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="37"/>
-      <c r="B65" s="38"/>
-      <c r="C65" s="30" t="s">
+      <c r="A65" s="29"/>
+      <c r="B65" s="30"/>
+      <c r="C65" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="D65" s="25" t="s">
+      <c r="D65" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E65" s="25">
+      <c r="E65" s="17">
         <v>24</v>
       </c>
-      <c r="F65" s="40"/>
-      <c r="G65" s="31"/>
-      <c r="H65" s="41"/>
+      <c r="F65" s="32"/>
+      <c r="G65" s="23"/>
+      <c r="H65" s="33"/>
     </row>
     <row r="66" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="37"/>
-      <c r="B66" s="38"/>
-      <c r="C66" s="30" t="s">
+      <c r="A66" s="29"/>
+      <c r="B66" s="30"/>
+      <c r="C66" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="D66" s="25" t="s">
+      <c r="D66" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="E66" s="25">
+      <c r="E66" s="17">
         <v>24</v>
       </c>
-      <c r="F66" s="40"/>
-      <c r="G66" s="31"/>
-      <c r="H66" s="41"/>
+      <c r="F66" s="32"/>
+      <c r="G66" s="23"/>
+      <c r="H66" s="33"/>
     </row>
     <row r="67" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="37"/>
-      <c r="B67" s="38"/>
-      <c r="C67" s="40" t="s">
+      <c r="A67" s="29"/>
+      <c r="B67" s="30"/>
+      <c r="C67" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="D67" s="40"/>
-      <c r="E67" s="40">
+      <c r="D67" s="32"/>
+      <c r="E67" s="32">
         <v>4</v>
       </c>
-      <c r="F67" s="40"/>
-      <c r="G67" s="31" t="s">
+      <c r="F67" s="32"/>
+      <c r="G67" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="H67" s="41">
+      <c r="H67" s="33">
         <v>24</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68" s="37"/>
-      <c r="B68" s="38"/>
-      <c r="C68" s="40"/>
-      <c r="D68" s="40"/>
-      <c r="E68" s="40"/>
-      <c r="F68" s="40"/>
-      <c r="G68" s="31" t="s">
+      <c r="A68" s="29"/>
+      <c r="B68" s="30"/>
+      <c r="C68" s="32"/>
+      <c r="D68" s="32"/>
+      <c r="E68" s="32"/>
+      <c r="F68" s="32"/>
+      <c r="G68" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H68" s="41"/>
+      <c r="H68" s="33"/>
     </row>
     <row r="69" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A69" s="32"/>
-      <c r="B69" s="33" t="s">
+      <c r="A69" s="24"/>
+      <c r="B69" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C69" s="34" t="s">
+      <c r="C69" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="D69" s="34"/>
-      <c r="E69" s="34"/>
-      <c r="F69" s="34"/>
-      <c r="G69" s="35"/>
-      <c r="H69" s="45" t="s">
+      <c r="D69" s="26"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="26"/>
+      <c r="G69" s="27"/>
+      <c r="H69" s="37" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A70" s="37"/>
-      <c r="B70" s="38"/>
-      <c r="C70" s="40" t="s">
+      <c r="A70" s="29"/>
+      <c r="B70" s="30"/>
+      <c r="C70" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="D70" s="40" t="s">
+      <c r="D70" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="E70" s="40">
+      <c r="E70" s="32">
         <v>9</v>
       </c>
-      <c r="F70" s="40" t="s">
+      <c r="F70" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="G70" s="31" t="s">
+      <c r="G70" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="H70" s="41">
+      <c r="H70" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="37"/>
-      <c r="B71" s="38"/>
-      <c r="C71" s="5" t="s">
+      <c r="A71" s="29"/>
+      <c r="B71" s="30"/>
+      <c r="C71" s="72" t="s">
         <v>75</v>
       </c>
-      <c r="D71" s="25" t="s">
+      <c r="D71" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E71" s="25">
+      <c r="E71" s="17">
         <v>1</v>
       </c>
-      <c r="F71" s="40"/>
-      <c r="G71" s="31">
+      <c r="F71" s="32"/>
+      <c r="G71" s="23">
         <v>10</v>
       </c>
-      <c r="H71" s="41">
+      <c r="H71" s="33">
         <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="37"/>
-      <c r="B72" s="38"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="40" t="s">
+      <c r="A72" s="29"/>
+      <c r="B72" s="30"/>
+      <c r="C72" s="72"/>
+      <c r="D72" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="E72" s="25">
+      <c r="E72" s="17">
         <v>7</v>
       </c>
-      <c r="F72" s="40"/>
-      <c r="G72" s="31" t="s">
+      <c r="F72" s="32"/>
+      <c r="G72" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="H72" s="41">
+      <c r="H72" s="33">
         <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="50"/>
-      <c r="B73" s="51"/>
-      <c r="C73" s="25" t="s">
+      <c r="A73" s="42"/>
+      <c r="B73" s="43"/>
+      <c r="C73" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D73" s="25" t="s">
+      <c r="D73" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E73" s="25">
+      <c r="E73" s="17">
         <v>15</v>
       </c>
-      <c r="F73" s="25" t="s">
+      <c r="F73" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="G73" s="31" t="s">
+      <c r="G73" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="H73" s="41">
+      <c r="H73" s="33">
         <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="37"/>
-      <c r="B74" s="38"/>
-      <c r="C74" s="40"/>
-      <c r="D74" s="40"/>
-      <c r="E74" s="40"/>
-      <c r="G74" s="31" t="s">
+      <c r="A74" s="29"/>
+      <c r="B74" s="30"/>
+      <c r="C74" s="32"/>
+      <c r="D74" s="32"/>
+      <c r="E74" s="32"/>
+      <c r="G74" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H74" s="41"/>
+      <c r="H74" s="33"/>
     </row>
     <row r="75" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="63"/>
-      <c r="B75" s="34" t="s">
+      <c r="A75" s="55"/>
+      <c r="B75" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="C75" s="34" t="s">
+      <c r="C75" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="D75" s="34"/>
-      <c r="E75" s="34"/>
-      <c r="F75" s="34"/>
-      <c r="G75" s="35"/>
-      <c r="H75" s="45" t="s">
+      <c r="D75" s="26"/>
+      <c r="E75" s="26"/>
+      <c r="F75" s="26"/>
+      <c r="G75" s="27"/>
+      <c r="H75" s="37" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="64"/>
-      <c r="C76" s="65" t="s">
+      <c r="A76" s="56"/>
+      <c r="C76" s="57" t="s">
         <v>136</v>
       </c>
-      <c r="D76" s="65"/>
-      <c r="E76" s="65">
+      <c r="D76" s="57"/>
+      <c r="E76" s="57">
         <v>10</v>
       </c>
-      <c r="F76" s="65"/>
-      <c r="G76" s="66" t="s">
+      <c r="F76" s="57"/>
+      <c r="G76" s="58" t="s">
         <v>137</v>
       </c>
-      <c r="H76" s="67">
+      <c r="H76" s="59">
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" s="68"/>
-      <c r="C77" s="2" t="s">
+      <c r="A77" s="60"/>
+      <c r="C77" s="73" t="s">
         <v>138</v>
       </c>
       <c r="D77" t="s">
@@ -2734,32 +2777,32 @@
       <c r="E77">
         <v>2</v>
       </c>
-      <c r="G77" s="69" t="s">
+      <c r="G77" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="H77" s="16">
+      <c r="H77" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="68"/>
-      <c r="C78" s="2"/>
+      <c r="A78" s="60"/>
+      <c r="C78" s="73"/>
       <c r="D78" t="s">
         <v>139</v>
       </c>
       <c r="E78">
         <v>10</v>
       </c>
-      <c r="G78" s="69" t="s">
+      <c r="G78" s="61" t="s">
         <v>140</v>
       </c>
-      <c r="H78" s="16">
+      <c r="H78" s="8">
         <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" s="68"/>
-      <c r="C79" s="2" t="s">
+      <c r="A79" s="60"/>
+      <c r="C79" s="73" t="s">
         <v>141</v>
       </c>
       <c r="D79" t="s">
@@ -2768,32 +2811,32 @@
       <c r="E79">
         <v>1</v>
       </c>
-      <c r="G79" s="69">
+      <c r="G79" s="61">
         <v>23</v>
       </c>
-      <c r="H79" s="16">
+      <c r="H79" s="8">
         <v>22</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="68"/>
-      <c r="C80" s="2"/>
+      <c r="A80" s="60"/>
+      <c r="C80" s="73"/>
       <c r="D80" t="s">
         <v>139</v>
       </c>
       <c r="E80">
         <v>5</v>
       </c>
-      <c r="G80" s="69" t="s">
+      <c r="G80" s="61" t="s">
         <v>142</v>
       </c>
-      <c r="H80" s="16">
+      <c r="H80" s="8">
         <v>23</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="68"/>
-      <c r="C81" s="70" t="s">
+      <c r="A81" s="60"/>
+      <c r="C81" s="62" t="s">
         <v>143</v>
       </c>
       <c r="D81" t="s">
@@ -2802,418 +2845,418 @@
       <c r="E81">
         <v>3</v>
       </c>
-      <c r="G81" s="69" t="s">
+      <c r="G81" s="61" t="s">
         <v>145</v>
       </c>
-      <c r="H81" s="16">
+      <c r="H81" s="8">
         <v>29</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="68"/>
-      <c r="C82" s="70"/>
-      <c r="G82" s="69"/>
-      <c r="H82" s="16"/>
+      <c r="A82" s="60"/>
+      <c r="C82" s="62"/>
+      <c r="G82" s="61"/>
+      <c r="H82" s="8"/>
     </row>
     <row r="83" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="32" t="s">
+      <c r="A83" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="B83" s="33" t="s">
+      <c r="B83" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C83" s="34" t="s">
+      <c r="C83" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="D83" s="34"/>
-      <c r="E83" s="34"/>
-      <c r="F83" s="34"/>
-      <c r="G83" s="35"/>
-      <c r="H83" s="45" t="s">
+      <c r="D83" s="26"/>
+      <c r="E83" s="26"/>
+      <c r="F83" s="26"/>
+      <c r="G83" s="27"/>
+      <c r="H83" s="37" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A84" s="37"/>
-      <c r="B84" s="38"/>
+      <c r="A84" s="29"/>
+      <c r="B84" s="30"/>
       <c r="C84" t="s">
         <v>149</v>
       </c>
-      <c r="D84" s="40"/>
-      <c r="E84" s="40">
+      <c r="D84" s="32"/>
+      <c r="E84" s="32">
         <v>4</v>
       </c>
-      <c r="F84" s="40" t="s">
+      <c r="F84" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="G84" s="31" t="s">
+      <c r="G84" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="H84" s="41">
+      <c r="H84" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A85" s="37"/>
-      <c r="B85" s="38"/>
-      <c r="C85" s="40" t="s">
+      <c r="A85" s="29"/>
+      <c r="B85" s="30"/>
+      <c r="C85" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="D85" s="40"/>
-      <c r="E85" s="40">
+      <c r="D85" s="32"/>
+      <c r="E85" s="32">
         <v>6</v>
       </c>
-      <c r="F85" s="40" t="s">
+      <c r="F85" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="G85" s="31" t="s">
+      <c r="G85" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="H85" s="41">
+      <c r="H85" s="33">
         <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="37"/>
-      <c r="B86" s="38"/>
-      <c r="C86" s="40" t="s">
+      <c r="A86" s="29"/>
+      <c r="B86" s="30"/>
+      <c r="C86" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="D86" s="40"/>
-      <c r="E86" s="40">
+      <c r="D86" s="32"/>
+      <c r="E86" s="32">
         <v>1</v>
       </c>
-      <c r="F86" s="40" t="s">
+      <c r="F86" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="G86" s="31">
+      <c r="G86" s="23">
         <v>11</v>
       </c>
-      <c r="H86" s="41">
+      <c r="H86" s="33">
         <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="37"/>
-      <c r="B87" s="38"/>
-      <c r="C87" s="40" t="s">
+      <c r="A87" s="29"/>
+      <c r="B87" s="30"/>
+      <c r="C87" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="D87" s="40"/>
-      <c r="E87" s="40">
+      <c r="D87" s="32"/>
+      <c r="E87" s="32">
         <v>6</v>
       </c>
-      <c r="F87" s="40" t="s">
+      <c r="F87" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="G87" s="31" t="s">
+      <c r="G87" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="H87" s="41">
+      <c r="H87" s="33">
         <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="37"/>
-      <c r="B88" s="38"/>
-      <c r="C88" s="40" t="s">
+      <c r="A88" s="29"/>
+      <c r="B88" s="30"/>
+      <c r="C88" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="D88" s="40"/>
-      <c r="E88" s="40">
+      <c r="D88" s="32"/>
+      <c r="E88" s="32">
         <v>1</v>
       </c>
-      <c r="F88" s="40" t="s">
+      <c r="F88" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="G88" s="31">
+      <c r="G88" s="23">
         <v>18</v>
       </c>
-      <c r="H88" s="41">
+      <c r="H88" s="33">
         <v>17</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A89" s="37"/>
-      <c r="B89" s="38"/>
-      <c r="C89" s="40" t="s">
+      <c r="A89" s="29"/>
+      <c r="B89" s="30"/>
+      <c r="C89" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="D89" s="40"/>
-      <c r="E89" s="40">
+      <c r="D89" s="32"/>
+      <c r="E89" s="32">
         <v>6</v>
       </c>
-      <c r="F89" s="40" t="s">
+      <c r="F89" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="G89" s="31" t="s">
+      <c r="G89" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="H89" s="41">
+      <c r="H89" s="33">
         <v>18</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A90" s="37"/>
-      <c r="B90" s="38"/>
-      <c r="C90" s="40" t="s">
+      <c r="A90" s="29"/>
+      <c r="B90" s="30"/>
+      <c r="C90" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="D90" s="40"/>
-      <c r="E90" s="40">
+      <c r="D90" s="32"/>
+      <c r="E90" s="32">
         <v>1</v>
       </c>
-      <c r="F90" s="40" t="s">
+      <c r="F90" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="G90" s="31">
+      <c r="G90" s="23">
         <v>25</v>
       </c>
-      <c r="H90" s="41">
+      <c r="H90" s="33">
         <v>24</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="37"/>
-      <c r="B91" s="38"/>
-      <c r="C91" s="40" t="s">
+      <c r="A91" s="29"/>
+      <c r="B91" s="30"/>
+      <c r="C91" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="D91" s="40"/>
-      <c r="E91" s="40">
+      <c r="D91" s="32"/>
+      <c r="E91" s="32">
         <v>6</v>
       </c>
-      <c r="F91" s="40" t="s">
+      <c r="F91" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="G91" s="31" t="s">
+      <c r="G91" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="H91" s="41">
+      <c r="H91" s="33">
         <v>25</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A92" s="37"/>
-      <c r="B92" s="38"/>
-      <c r="C92" s="40" t="s">
+      <c r="A92" s="29"/>
+      <c r="B92" s="30"/>
+      <c r="C92" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="D92" s="40"/>
-      <c r="E92" s="40">
+      <c r="D92" s="32"/>
+      <c r="E92" s="32">
         <v>1</v>
       </c>
-      <c r="F92" s="40" t="s">
+      <c r="F92" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="G92" s="31">
+      <c r="G92" s="23">
         <v>32</v>
       </c>
-      <c r="H92" s="41">
+      <c r="H92" s="33">
         <v>31</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93" s="37"/>
-      <c r="B93" s="38"/>
-      <c r="C93" s="40"/>
-      <c r="D93" s="40"/>
-      <c r="E93" s="40"/>
-      <c r="F93" s="40"/>
-      <c r="G93" s="31"/>
-      <c r="H93" s="41"/>
+      <c r="A93" s="29"/>
+      <c r="B93" s="30"/>
+      <c r="C93" s="32"/>
+      <c r="D93" s="32"/>
+      <c r="E93" s="32"/>
+      <c r="F93" s="32"/>
+      <c r="G93" s="23"/>
+      <c r="H93" s="33"/>
     </row>
     <row r="94" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A94" s="32" t="s">
+      <c r="A94" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="B94" s="33" t="s">
+      <c r="B94" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="C94" s="34" t="s">
+      <c r="C94" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="D94" s="34"/>
-      <c r="E94" s="34"/>
-      <c r="F94" s="34"/>
-      <c r="G94" s="35" t="s">
+      <c r="D94" s="26"/>
+      <c r="E94" s="26"/>
+      <c r="F94" s="26"/>
+      <c r="G94" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="H94" s="45" t="s">
+      <c r="H94" s="37" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A95" s="37"/>
-      <c r="B95" s="38"/>
-      <c r="C95" s="5" t="s">
+      <c r="A95" s="29"/>
+      <c r="B95" s="30"/>
+      <c r="C95" s="72" t="s">
         <v>167</v>
       </c>
-      <c r="D95" s="25" t="s">
+      <c r="D95" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E95" s="40">
+      <c r="E95" s="32">
         <v>1</v>
       </c>
-      <c r="F95" s="40"/>
-      <c r="G95" s="31">
+      <c r="F95" s="32"/>
+      <c r="G95" s="23">
         <v>1</v>
       </c>
-      <c r="H95" s="41">
+      <c r="H95" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A96" s="37"/>
-      <c r="B96" s="38"/>
-      <c r="C96" s="5"/>
-      <c r="D96" s="40" t="s">
+      <c r="A96" s="29"/>
+      <c r="B96" s="30"/>
+      <c r="C96" s="72"/>
+      <c r="D96" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="E96" s="40">
+      <c r="E96" s="32">
         <v>7</v>
       </c>
-      <c r="F96" s="40"/>
-      <c r="G96" s="31" t="s">
+      <c r="F96" s="32"/>
+      <c r="G96" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="H96" s="41">
+      <c r="H96" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A97" s="37"/>
-      <c r="B97" s="38"/>
-      <c r="C97" s="40" t="s">
+      <c r="A97" s="29"/>
+      <c r="B97" s="30"/>
+      <c r="C97" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="D97" s="40"/>
-      <c r="E97" s="40">
+      <c r="D97" s="32"/>
+      <c r="E97" s="32">
         <v>7</v>
       </c>
-      <c r="F97" s="40" t="s">
+      <c r="F97" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="G97" s="31" t="s">
+      <c r="G97" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="H97" s="41">
+      <c r="H97" s="33">
         <v>8</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A98" s="37"/>
-      <c r="B98" s="38"/>
-      <c r="C98" s="5" t="s">
+      <c r="A98" s="29"/>
+      <c r="B98" s="30"/>
+      <c r="C98" s="72" t="s">
         <v>171</v>
       </c>
-      <c r="D98" s="25" t="s">
+      <c r="D98" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E98" s="40">
+      <c r="E98" s="32">
         <v>2</v>
       </c>
-      <c r="F98" s="40"/>
-      <c r="G98" s="31" t="s">
+      <c r="F98" s="32"/>
+      <c r="G98" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="H98" s="41">
+      <c r="H98" s="33">
         <v>15</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A99" s="37"/>
-      <c r="B99" s="38"/>
-      <c r="C99" s="5"/>
-      <c r="D99" s="40" t="s">
+      <c r="A99" s="29"/>
+      <c r="B99" s="30"/>
+      <c r="C99" s="72"/>
+      <c r="D99" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="E99" s="40">
+      <c r="E99" s="32">
         <v>10</v>
       </c>
-      <c r="F99" s="40"/>
-      <c r="G99" s="31" t="s">
+      <c r="F99" s="32"/>
+      <c r="G99" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="H99" s="41">
+      <c r="H99" s="33">
         <v>17</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A100" s="37"/>
-      <c r="B100" s="38"/>
-      <c r="C100" s="5"/>
-      <c r="D100" s="40" t="s">
+      <c r="A100" s="29"/>
+      <c r="B100" s="30"/>
+      <c r="C100" s="72"/>
+      <c r="D100" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="E100" s="40">
+      <c r="E100" s="32">
         <v>1</v>
       </c>
-      <c r="F100" s="54"/>
-      <c r="G100" s="31">
+      <c r="F100" s="46"/>
+      <c r="G100" s="23">
         <v>28</v>
       </c>
-      <c r="H100" s="41">
+      <c r="H100" s="33">
         <v>27</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" s="68"/>
-      <c r="G101" s="69"/>
-      <c r="H101" s="16"/>
+      <c r="A101" s="60"/>
+      <c r="G101" s="61"/>
+      <c r="H101" s="8"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" s="71"/>
-      <c r="B102" s="72" t="s">
+      <c r="A102" s="63"/>
+      <c r="B102" s="64" t="s">
         <v>174</v>
       </c>
-      <c r="C102" s="72" t="s">
+      <c r="C102" s="64" t="s">
         <v>175</v>
       </c>
-      <c r="D102" s="72"/>
-      <c r="E102" s="72"/>
-      <c r="F102" s="72"/>
-      <c r="G102" s="73"/>
-      <c r="H102" s="74"/>
+      <c r="D102" s="64"/>
+      <c r="E102" s="64"/>
+      <c r="F102" s="64"/>
+      <c r="G102" s="65"/>
+      <c r="H102" s="66"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="64"/>
-      <c r="B103" s="65"/>
-      <c r="C103" s="1" t="s">
+      <c r="A103" s="56"/>
+      <c r="B103" s="57"/>
+      <c r="C103" s="71" t="s">
         <v>176</v>
       </c>
       <c r="D103" t="s">
         <v>57</v>
       </c>
-      <c r="E103" s="65">
+      <c r="E103" s="57">
         <v>1</v>
       </c>
-      <c r="F103" s="65"/>
-      <c r="G103" s="66">
+      <c r="F103" s="57"/>
+      <c r="G103" s="58">
         <v>1</v>
       </c>
-      <c r="H103" s="67">
+      <c r="H103" s="59">
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="68"/>
-      <c r="C104" s="1"/>
+      <c r="A104" s="60"/>
+      <c r="C104" s="71"/>
       <c r="D104" t="s">
         <v>177</v>
       </c>
       <c r="E104">
         <v>7</v>
       </c>
-      <c r="G104" s="69" t="s">
+      <c r="G104" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="H104" s="16">
+      <c r="H104" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="68"/>
+      <c r="A105" s="60"/>
       <c r="C105" t="s">
         <v>178</v>
       </c>
@@ -3223,41 +3266,41 @@
       <c r="E105">
         <v>7</v>
       </c>
-      <c r="G105" s="69" t="s">
+      <c r="G105" s="61" t="s">
         <v>170</v>
       </c>
-      <c r="H105" s="16">
+      <c r="H105" s="8">
         <v>8</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="75"/>
-      <c r="B106" s="76"/>
-      <c r="C106" s="76"/>
-      <c r="D106" s="76"/>
-      <c r="E106" s="76"/>
-      <c r="F106" s="76"/>
-      <c r="G106" s="77"/>
-      <c r="H106" s="78"/>
+      <c r="A106" s="67"/>
+      <c r="B106" s="68"/>
+      <c r="C106" s="68"/>
+      <c r="D106" s="68"/>
+      <c r="E106" s="68"/>
+      <c r="F106" s="68"/>
+      <c r="G106" s="69"/>
+      <c r="H106" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C57:C58"/>
     <mergeCell ref="C103:C104"/>
     <mergeCell ref="C71:C72"/>
     <mergeCell ref="C77:C78"/>
     <mergeCell ref="C79:C80"/>
     <mergeCell ref="C95:C96"/>
     <mergeCell ref="C98:C100"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="C34:C35"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>